<commit_message>
Adding extra comment and Master code to report
</commit_message>
<xml_diff>
--- a/SmartKitchen-Emdebbed System/Documents/Parts and needs/Farnel-list.xlsx
+++ b/SmartKitchen-Emdebbed System/Documents/Parts and needs/Farnel-list.xlsx
@@ -305,7 +305,7 @@
     <t xml:space="preserve">To read products </t>
   </si>
   <si>
-    <t>Component list:</t>
+    <t xml:space="preserve"> Supplementary component list:</t>
   </si>
 </sst>
 </file>
@@ -368,7 +368,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -540,6 +540,32 @@
         <color auto="1"/>
       </top>
       <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -565,8 +591,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -585,6 +609,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -994,7 +1020,7 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="F36" sqref="A2:F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1008,17 +1034,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="13"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="11"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="17" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="7" t="s">
@@ -1033,7 +1059,7 @@
       <c r="E2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="18" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1678,7 +1704,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="17">
+      <c r="A35" s="15">
         <v>33</v>
       </c>
       <c r="B35" s="8" t="s">
@@ -1698,26 +1724,26 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="9"/>
-      <c r="B36" s="10"/>
-      <c r="C36" s="15" t="s">
+      <c r="A36" s="19"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="D36" s="18">
+      <c r="D36" s="16">
         <f>SUBTOTAL(109,D3:D35)</f>
         <v>314</v>
       </c>
-      <c r="E36" s="15" t="s">
+      <c r="E36" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="F36" s="16">
+      <c r="F36" s="14">
         <f>SUBTOTAL(109,F3:F35)</f>
         <v>224.82000000000002</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="14"/>
-      <c r="B37" s="14"/>
+      <c r="A37" s="12"/>
+      <c r="B37" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>